<commit_message>
extended all for figure 4
</commit_message>
<xml_diff>
--- a/documentation/figure_4/figure_4.xlsx
+++ b/documentation/figure_4/figure_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrencetang/Desktop/Internships:Research/UROP/oilresearch/documentation/figure_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD27660-10EC-114B-8162-38A446F0746D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BECC48-768F-E040-8F97-60363067C23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
+    <workbookView xWindow="820" yWindow="1620" windowWidth="18120" windowHeight="18880" activeTab="6" xr2:uid="{0CDE113E-35AD-2643-904C-47F0C01455AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="5" r:id="rId1"/>
@@ -290,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,6 +390,19 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -413,7 +426,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -471,6 +484,9 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13773,7 +13789,7 @@
                   <c:v>-22.225999999999999</c:v>
                 </c:pt>
                 <c:pt idx="531">
-                  <c:v>-22.66</c:v>
+                  <c:v>-22.742000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26762,11 +26778,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C491D87-F346-CA48-BF83-3B74F4392A2D}">
-  <dimension ref="A1:I563"/>
+  <dimension ref="A1:I602"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A578" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K562" sqref="K562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37109,11 +37125,11 @@
         <v>79.66</v>
       </c>
       <c r="D521" s="6">
-        <f t="shared" ref="D521:D563" si="16">B521-C521</f>
+        <f t="shared" ref="D521:D566" si="16">B521-C521</f>
         <v>-12.530000000000001</v>
       </c>
       <c r="E521" s="30">
-        <f t="shared" ref="E521:E563" si="17" xml:space="preserve"> ROUND(AVERAGE(D517:D521),3)</f>
+        <f t="shared" ref="E521:E584" si="17" xml:space="preserve"> ROUND(AVERAGE(D517:D521),3)</f>
         <v>-12.35</v>
       </c>
       <c r="F521" s="4"/>
@@ -37928,6 +37944,571 @@
         <f t="shared" si="17"/>
         <v>-11.91</v>
       </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A564" s="20">
+        <v>45342</v>
+      </c>
+      <c r="B564" s="4">
+        <v>70.87</v>
+      </c>
+      <c r="C564" s="6">
+        <v>82.34</v>
+      </c>
+      <c r="D564" s="6">
+        <f t="shared" si="16"/>
+        <v>-11.469999999999999</v>
+      </c>
+      <c r="E564" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.792</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A565" s="20">
+        <v>45343</v>
+      </c>
+      <c r="B565" s="4">
+        <v>71.39</v>
+      </c>
+      <c r="C565" s="6">
+        <v>83.02</v>
+      </c>
+      <c r="D565" s="6">
+        <f t="shared" si="16"/>
+        <v>-11.629999999999995</v>
+      </c>
+      <c r="E565" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.714</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A566" s="20">
+        <v>45344</v>
+      </c>
+      <c r="B566" s="4">
+        <v>71.56</v>
+      </c>
+      <c r="C566" s="6">
+        <v>83.67</v>
+      </c>
+      <c r="D566" s="6">
+        <f t="shared" si="16"/>
+        <v>-12.11</v>
+      </c>
+      <c r="E566" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.746</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A567" s="20">
+        <v>45345</v>
+      </c>
+      <c r="B567" s="4">
+        <v>69.739999999999995</v>
+      </c>
+      <c r="C567" s="6">
+        <v>81.62</v>
+      </c>
+      <c r="D567" s="6">
+        <f>B567-C567</f>
+        <v>-11.88000000000001</v>
+      </c>
+      <c r="E567" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.77</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A568" s="20">
+        <v>45348</v>
+      </c>
+      <c r="B568" s="4">
+        <v>70.53</v>
+      </c>
+      <c r="C568" s="6">
+        <v>82.53</v>
+      </c>
+      <c r="D568" s="6">
+        <f t="shared" ref="D568:D591" si="18">B568-C568</f>
+        <v>-12</v>
+      </c>
+      <c r="E568" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.818</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A569" s="20">
+        <v>45349</v>
+      </c>
+      <c r="B569" s="4">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="C569" s="6">
+        <v>83.65</v>
+      </c>
+      <c r="D569" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.300000000000011</v>
+      </c>
+      <c r="E569" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.984</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A570" s="20">
+        <v>45350</v>
+      </c>
+      <c r="B570" s="4">
+        <v>70.959999999999994</v>
+      </c>
+      <c r="C570" s="6">
+        <v>83.68</v>
+      </c>
+      <c r="D570" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.720000000000013</v>
+      </c>
+      <c r="E570" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.202</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A571" s="20">
+        <v>45351</v>
+      </c>
+      <c r="B571" s="4">
+        <v>71.58</v>
+      </c>
+      <c r="C571" s="6">
+        <v>83.62</v>
+      </c>
+      <c r="D571" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.040000000000006</v>
+      </c>
+      <c r="E571" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.188000000000001</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A572" s="20">
+        <v>45352</v>
+      </c>
+      <c r="B572" s="4">
+        <v>71.47</v>
+      </c>
+      <c r="C572" s="6">
+        <v>83.55</v>
+      </c>
+      <c r="D572" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.079999999999998</v>
+      </c>
+      <c r="E572" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.228</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A573" s="20">
+        <v>45355</v>
+      </c>
+      <c r="B573" s="4">
+        <v>70.89</v>
+      </c>
+      <c r="C573" s="6">
+        <v>82.8</v>
+      </c>
+      <c r="D573" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.909999999999997</v>
+      </c>
+      <c r="E573" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.21</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A574" s="20">
+        <v>45356</v>
+      </c>
+      <c r="B574" s="4">
+        <v>70.010000000000005</v>
+      </c>
+      <c r="C574" s="31">
+        <v>82.04</v>
+      </c>
+      <c r="D574" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.030000000000001</v>
+      </c>
+      <c r="E574" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.156000000000001</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A575" s="20">
+        <v>45357</v>
+      </c>
+      <c r="B575" s="4">
+        <v>70.92</v>
+      </c>
+      <c r="C575" s="31">
+        <v>82.96</v>
+      </c>
+      <c r="D575" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.039999999999992</v>
+      </c>
+      <c r="E575" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.02</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A576" s="20">
+        <v>45358</v>
+      </c>
+      <c r="B576" s="4">
+        <v>71.38</v>
+      </c>
+      <c r="C576" s="31">
+        <v>82.96</v>
+      </c>
+      <c r="D576" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.579999999999998</v>
+      </c>
+      <c r="E576" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.928000000000001</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A577" s="20">
+        <v>45359</v>
+      </c>
+      <c r="B577" s="4">
+        <v>69.98</v>
+      </c>
+      <c r="C577" s="31">
+        <v>82.08</v>
+      </c>
+      <c r="D577" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.099999999999994</v>
+      </c>
+      <c r="E577" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.932</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A578" s="20">
+        <v>45362</v>
+      </c>
+      <c r="B578" s="4">
+        <v>70.33</v>
+      </c>
+      <c r="C578" s="31">
+        <v>82.21</v>
+      </c>
+      <c r="D578" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.879999999999995</v>
+      </c>
+      <c r="E578" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.926</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A579" s="20">
+        <v>45363</v>
+      </c>
+      <c r="B579" s="4">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="C579" s="31">
+        <v>81.92</v>
+      </c>
+      <c r="D579" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.659999999999997</v>
+      </c>
+      <c r="E579" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.852</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A580" s="20">
+        <v>45364</v>
+      </c>
+      <c r="B580" s="4">
+        <v>71.790000000000006</v>
+      </c>
+      <c r="C580" s="31">
+        <v>84.03</v>
+      </c>
+      <c r="D580" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.239999999999995</v>
+      </c>
+      <c r="E580" s="30">
+        <f t="shared" si="17"/>
+        <v>-11.891999999999999</v>
+      </c>
+    </row>
+    <row r="581" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A581" s="20">
+        <v>45365</v>
+      </c>
+      <c r="B581" s="4">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="C581" s="31">
+        <v>85.42</v>
+      </c>
+      <c r="D581" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.320000000000007</v>
+      </c>
+      <c r="E581" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.04</v>
+      </c>
+    </row>
+    <row r="582" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A582" s="20">
+        <v>45366</v>
+      </c>
+      <c r="B582" s="4">
+        <v>73.27</v>
+      </c>
+      <c r="C582" s="31">
+        <v>85.34</v>
+      </c>
+      <c r="D582" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.070000000000007</v>
+      </c>
+      <c r="E582" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.034000000000001</v>
+      </c>
+    </row>
+    <row r="583" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A583" s="20">
+        <v>45369</v>
+      </c>
+      <c r="B583" s="4">
+        <v>74.7</v>
+      </c>
+      <c r="C583" s="31">
+        <v>86.89</v>
+      </c>
+      <c r="D583" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.189999999999998</v>
+      </c>
+      <c r="E583" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.096</v>
+      </c>
+    </row>
+    <row r="584" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A584" s="20">
+        <v>45370</v>
+      </c>
+      <c r="B584" s="4">
+        <v>75.069999999999993</v>
+      </c>
+      <c r="C584" s="31">
+        <v>87.38</v>
+      </c>
+      <c r="D584" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.310000000000002</v>
+      </c>
+      <c r="E584" s="30">
+        <f t="shared" si="17"/>
+        <v>-12.226000000000001</v>
+      </c>
+    </row>
+    <row r="585" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A585" s="20">
+        <v>45371</v>
+      </c>
+      <c r="B585" s="4">
+        <v>74.010000000000005</v>
+      </c>
+      <c r="C585" s="31">
+        <v>85.95</v>
+      </c>
+      <c r="D585" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.939999999999998</v>
+      </c>
+      <c r="E585" s="30">
+        <f t="shared" ref="E585:E591" si="19" xml:space="preserve"> ROUND(AVERAGE(D581:D585),3)</f>
+        <v>-12.166</v>
+      </c>
+    </row>
+    <row r="586" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A586" s="20">
+        <v>45372</v>
+      </c>
+      <c r="B586" s="4">
+        <v>73.38</v>
+      </c>
+      <c r="C586" s="31">
+        <v>85.78</v>
+      </c>
+      <c r="D586" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.400000000000006</v>
+      </c>
+      <c r="E586" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.182</v>
+      </c>
+    </row>
+    <row r="587" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A587" s="20">
+        <v>45373</v>
+      </c>
+      <c r="B587" s="4">
+        <v>73.459999999999994</v>
+      </c>
+      <c r="C587" s="31">
+        <v>85.43</v>
+      </c>
+      <c r="D587" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.970000000000013</v>
+      </c>
+      <c r="E587" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.162000000000001</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A588" s="20">
+        <v>45376</v>
+      </c>
+      <c r="B588" s="4">
+        <v>74.41</v>
+      </c>
+      <c r="C588" s="31">
+        <v>86.75</v>
+      </c>
+      <c r="D588" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.340000000000003</v>
+      </c>
+      <c r="E588" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.192</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A589" s="20">
+        <v>45377</v>
+      </c>
+      <c r="B589" s="4">
+        <v>73.680000000000007</v>
+      </c>
+      <c r="C589" s="31">
+        <v>86.25</v>
+      </c>
+      <c r="D589" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.569999999999993</v>
+      </c>
+      <c r="E589" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.244</v>
+      </c>
+    </row>
+    <row r="590" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A590" s="20">
+        <v>45378</v>
+      </c>
+      <c r="B590" s="4">
+        <v>73.94</v>
+      </c>
+      <c r="C590" s="31">
+        <v>86.09</v>
+      </c>
+      <c r="D590" s="6">
+        <f t="shared" si="18"/>
+        <v>-12.150000000000006</v>
+      </c>
+      <c r="E590" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.286</v>
+      </c>
+    </row>
+    <row r="591" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A591" s="20">
+        <v>45379</v>
+      </c>
+      <c r="B591" s="4">
+        <v>75.540000000000006</v>
+      </c>
+      <c r="C591" s="31">
+        <v>87.48</v>
+      </c>
+      <c r="D591" s="6">
+        <f t="shared" si="18"/>
+        <v>-11.939999999999998</v>
+      </c>
+      <c r="E591" s="30">
+        <f t="shared" si="19"/>
+        <v>-12.194000000000001</v>
+      </c>
+    </row>
+    <row r="592" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="C592" s="31"/>
+    </row>
+    <row r="593" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C593" s="31"/>
+    </row>
+    <row r="594" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C594" s="31"/>
+    </row>
+    <row r="595" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C595" s="31"/>
+    </row>
+    <row r="596" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C596" s="31"/>
+    </row>
+    <row r="597" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C597" s="31"/>
+    </row>
+    <row r="598" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C598" s="31"/>
+    </row>
+    <row r="599" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C599" s="31"/>
+    </row>
+    <row r="600" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C600" s="31"/>
+    </row>
+    <row r="601" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C601" s="31"/>
+    </row>
+    <row r="602" spans="3:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="C602" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -61245,11 +61826,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC841A3D-0425-7F4C-9464-9A4518464EF5}">
-  <dimension ref="A1:K541"/>
+  <dimension ref="A1:K600"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8:I539"/>
+      <pane ySplit="7" topLeftCell="A563" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A539" sqref="A539:A599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -77278,11 +77859,11 @@
         <v>79.34</v>
       </c>
       <c r="H521" s="4">
-        <f t="shared" ref="H521:H539" si="16">AVERAGE(C521,F521)-G521</f>
+        <f t="shared" ref="H521:H584" si="16">AVERAGE(C521,F521)-G521</f>
         <v>-20.64</v>
       </c>
       <c r="I521">
-        <f t="shared" ref="I521:I539" si="17" xml:space="preserve"> ROUND(AVERAGE(H517:H521), 3)</f>
+        <f t="shared" ref="I521:I584" si="17" xml:space="preserve"> ROUND(AVERAGE(H517:H521), 3)</f>
         <v>-21.411999999999999</v>
       </c>
     </row>
@@ -77814,41 +78395,1902 @@
       </c>
     </row>
     <row r="539" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A539" s="2">
+      <c r="A539" s="33">
         <v>45307</v>
       </c>
-      <c r="B539">
-        <v>61.76</v>
-      </c>
-      <c r="C539">
+      <c r="B539" s="32">
+        <v>62.15</v>
+      </c>
+      <c r="C539" s="32">
         <v>55.61</v>
       </c>
-      <c r="D539">
-        <v>61.76</v>
-      </c>
-      <c r="E539">
-        <v>60.76</v>
-      </c>
-      <c r="F539">
+      <c r="D539" s="32">
+        <v>62.15</v>
+      </c>
+      <c r="E539" s="32">
+        <v>61.15</v>
+      </c>
+      <c r="F539" s="32">
         <v>55.61</v>
       </c>
-      <c r="G539">
-        <v>77.94</v>
+      <c r="G539" s="32">
+        <v>78.349999999999994</v>
       </c>
       <c r="H539" s="4">
         <f t="shared" si="16"/>
-        <v>-22.33</v>
+        <v>-22.739999999999995</v>
       </c>
       <c r="I539">
         <f t="shared" si="17"/>
-        <v>-22.66</v>
+        <v>-22.742000000000001</v>
       </c>
     </row>
     <row r="540" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H540" s="4"/>
+      <c r="A540" s="33">
+        <v>45308</v>
+      </c>
+      <c r="B540" s="32">
+        <v>60.89</v>
+      </c>
+      <c r="C540" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="D540" s="32">
+        <v>60.89</v>
+      </c>
+      <c r="E540" s="32">
+        <v>59.89</v>
+      </c>
+      <c r="F540" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="G540" s="32">
+        <v>77.62</v>
+      </c>
+      <c r="H540" s="4">
+        <f t="shared" si="16"/>
+        <v>-22.010000000000005</v>
+      </c>
+      <c r="I540">
+        <f t="shared" si="17"/>
+        <v>-22.776</v>
+      </c>
     </row>
     <row r="541" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H541" s="4"/>
+      <c r="A541" s="33">
+        <v>45309</v>
+      </c>
+      <c r="B541" s="32">
+        <v>63.04</v>
+      </c>
+      <c r="C541" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="D541" s="32">
+        <v>63.04</v>
+      </c>
+      <c r="E541" s="32">
+        <v>62.04</v>
+      </c>
+      <c r="F541" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="G541" s="32">
+        <v>78.709999999999994</v>
+      </c>
+      <c r="H541" s="4">
+        <f t="shared" si="16"/>
+        <v>-23.099999999999994</v>
+      </c>
+      <c r="I541">
+        <f t="shared" si="17"/>
+        <v>-22.716000000000001</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A542" s="33">
+        <v>45310</v>
+      </c>
+      <c r="B542" s="32">
+        <v>62.71</v>
+      </c>
+      <c r="C542" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="D542" s="32">
+        <v>62.71</v>
+      </c>
+      <c r="E542" s="32">
+        <v>61.71</v>
+      </c>
+      <c r="F542" s="32">
+        <v>55.61</v>
+      </c>
+      <c r="G542" s="32">
+        <v>79.09</v>
+      </c>
+      <c r="H542" s="4">
+        <f t="shared" si="16"/>
+        <v>-23.480000000000004</v>
+      </c>
+      <c r="I542">
+        <f t="shared" si="17"/>
+        <v>-22.731999999999999</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A543" s="33">
+        <v>45313</v>
+      </c>
+      <c r="B543" s="32">
+        <v>63.7</v>
+      </c>
+      <c r="C543" s="32">
+        <v>62.9</v>
+      </c>
+      <c r="D543" s="32">
+        <v>63.7</v>
+      </c>
+      <c r="E543" s="32">
+        <v>62.7</v>
+      </c>
+      <c r="F543" s="32">
+        <v>62.9</v>
+      </c>
+      <c r="G543" s="32">
+        <v>80.010000000000005</v>
+      </c>
+      <c r="H543" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.110000000000007</v>
+      </c>
+      <c r="I543">
+        <f t="shared" si="17"/>
+        <v>-21.687999999999999</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A544" s="33">
+        <v>45314</v>
+      </c>
+      <c r="B544" s="32">
+        <v>71.48</v>
+      </c>
+      <c r="C544" s="32">
+        <v>63.24</v>
+      </c>
+      <c r="D544" s="32">
+        <v>71.48</v>
+      </c>
+      <c r="E544" s="32">
+        <v>67.69</v>
+      </c>
+      <c r="F544" s="32">
+        <v>63.24</v>
+      </c>
+      <c r="G544" s="32">
+        <v>80.22</v>
+      </c>
+      <c r="H544" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.979999999999997</v>
+      </c>
+      <c r="I544">
+        <f t="shared" si="17"/>
+        <v>-20.536000000000001</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A545" s="33">
+        <v>45315</v>
+      </c>
+      <c r="B545" s="32">
+        <v>71.52</v>
+      </c>
+      <c r="C545" s="32">
+        <v>63.36</v>
+      </c>
+      <c r="D545" s="32">
+        <v>71.52</v>
+      </c>
+      <c r="E545" s="32">
+        <v>67.8</v>
+      </c>
+      <c r="F545" s="32">
+        <v>63.36</v>
+      </c>
+      <c r="G545" s="32">
+        <v>80.33</v>
+      </c>
+      <c r="H545" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.97</v>
+      </c>
+      <c r="I545">
+        <f t="shared" si="17"/>
+        <v>-19.527999999999999</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A546" s="33">
+        <v>45316</v>
+      </c>
+      <c r="B546" s="32">
+        <v>71.63</v>
+      </c>
+      <c r="C546" s="32">
+        <v>63.53</v>
+      </c>
+      <c r="D546" s="32">
+        <v>71.63</v>
+      </c>
+      <c r="E546" s="32">
+        <v>68.09</v>
+      </c>
+      <c r="F546" s="32">
+        <v>63.53</v>
+      </c>
+      <c r="G546" s="32">
+        <v>81.34</v>
+      </c>
+      <c r="H546" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.810000000000002</v>
+      </c>
+      <c r="I546">
+        <f t="shared" si="17"/>
+        <v>-18.47</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A547" s="33">
+        <v>45317</v>
+      </c>
+      <c r="B547" s="32">
+        <v>72.61</v>
+      </c>
+      <c r="C547" s="32">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="D547" s="32">
+        <v>72.61</v>
+      </c>
+      <c r="E547" s="32">
+        <v>68.959999999999994</v>
+      </c>
+      <c r="F547" s="32">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="G547" s="32">
+        <v>81.95</v>
+      </c>
+      <c r="H547" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.409999999999997</v>
+      </c>
+      <c r="I547">
+        <f t="shared" si="17"/>
+        <v>-17.256</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A548" s="33">
+        <v>45320</v>
+      </c>
+      <c r="B548" s="32">
+        <v>73.260000000000005</v>
+      </c>
+      <c r="C548" s="32">
+        <v>65.19</v>
+      </c>
+      <c r="D548" s="32">
+        <v>73.260000000000005</v>
+      </c>
+      <c r="E548" s="32">
+        <v>69.61</v>
+      </c>
+      <c r="F548" s="32">
+        <v>65.19</v>
+      </c>
+      <c r="G548" s="32">
+        <v>82.69</v>
+      </c>
+      <c r="H548" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.5</v>
+      </c>
+      <c r="I548">
+        <f t="shared" si="17"/>
+        <v>-17.334</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A549" s="33">
+        <v>45321</v>
+      </c>
+      <c r="B549" s="32">
+        <v>73.39</v>
+      </c>
+      <c r="C549" s="32">
+        <v>65.19</v>
+      </c>
+      <c r="D549" s="32">
+        <v>73.39</v>
+      </c>
+      <c r="E549" s="32">
+        <v>69.739999999999995</v>
+      </c>
+      <c r="F549" s="32">
+        <v>65.19</v>
+      </c>
+      <c r="G549" s="32">
+        <v>82.83</v>
+      </c>
+      <c r="H549" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.64</v>
+      </c>
+      <c r="I549">
+        <f t="shared" si="17"/>
+        <v>-17.466000000000001</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A550" s="33">
+        <v>45322</v>
+      </c>
+      <c r="B550" s="32">
+        <v>72.209999999999994</v>
+      </c>
+      <c r="C550" s="32">
+        <v>65.34</v>
+      </c>
+      <c r="D550" s="32">
+        <v>72.209999999999994</v>
+      </c>
+      <c r="E550" s="32">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="F550" s="32">
+        <v>65.34</v>
+      </c>
+      <c r="G550" s="32">
+        <v>81.93</v>
+      </c>
+      <c r="H550" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.590000000000003</v>
+      </c>
+      <c r="I550">
+        <f t="shared" si="17"/>
+        <v>-17.39</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A551" s="33">
+        <v>45323</v>
+      </c>
+      <c r="B551" s="32">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="C551" s="32">
+        <v>63.4</v>
+      </c>
+      <c r="D551" s="32">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="E551" s="32">
+        <v>67.819999999999993</v>
+      </c>
+      <c r="F551" s="32">
+        <v>63.4</v>
+      </c>
+      <c r="G551" s="32">
+        <v>81.5</v>
+      </c>
+      <c r="H551" s="4">
+        <f t="shared" si="16"/>
+        <v>-18.100000000000001</v>
+      </c>
+      <c r="I551">
+        <f t="shared" si="17"/>
+        <v>-17.448</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A552" s="33">
+        <v>45324</v>
+      </c>
+      <c r="B552" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="C552" s="32">
+        <v>60.74</v>
+      </c>
+      <c r="D552" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="E552" s="32">
+        <v>65.16</v>
+      </c>
+      <c r="F552" s="32">
+        <v>60.74</v>
+      </c>
+      <c r="G552" s="32">
+        <v>77.53</v>
+      </c>
+      <c r="H552" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.79</v>
+      </c>
+      <c r="I552">
+        <f t="shared" si="17"/>
+        <v>-17.324000000000002</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A553" s="33">
+        <v>45327</v>
+      </c>
+      <c r="B553" s="32">
+        <v>68.53</v>
+      </c>
+      <c r="C553" s="32">
+        <v>60.5</v>
+      </c>
+      <c r="D553" s="32">
+        <v>68.53</v>
+      </c>
+      <c r="E553" s="32">
+        <v>64.92</v>
+      </c>
+      <c r="F553" s="32">
+        <v>60.5</v>
+      </c>
+      <c r="G553" s="32">
+        <v>77.28</v>
+      </c>
+      <c r="H553" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.78</v>
+      </c>
+      <c r="I553">
+        <f t="shared" si="17"/>
+        <v>-17.18</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A554" s="33">
+        <v>45328</v>
+      </c>
+      <c r="B554" s="32">
+        <v>69.66</v>
+      </c>
+      <c r="C554" s="32">
+        <v>61.66</v>
+      </c>
+      <c r="D554" s="32">
+        <v>69.66</v>
+      </c>
+      <c r="E554" s="32">
+        <v>65.84</v>
+      </c>
+      <c r="F554" s="32">
+        <v>61.66</v>
+      </c>
+      <c r="G554" s="32">
+        <v>78.7</v>
+      </c>
+      <c r="H554" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.040000000000006</v>
+      </c>
+      <c r="I554">
+        <f t="shared" si="17"/>
+        <v>-17.059999999999999</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A555" s="33">
+        <v>45329</v>
+      </c>
+      <c r="B555" s="32">
+        <v>70.38</v>
+      </c>
+      <c r="C555" s="32">
+        <v>62.38</v>
+      </c>
+      <c r="D555" s="32">
+        <v>70.38</v>
+      </c>
+      <c r="E555" s="32">
+        <v>66.56</v>
+      </c>
+      <c r="F555" s="32">
+        <v>62.38</v>
+      </c>
+      <c r="G555" s="32">
+        <v>79.19</v>
+      </c>
+      <c r="H555" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.809999999999995</v>
+      </c>
+      <c r="I555">
+        <f t="shared" si="17"/>
+        <v>-17.103999999999999</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A556" s="33">
+        <v>45330</v>
+      </c>
+      <c r="B556" s="32">
+        <v>72.209999999999994</v>
+      </c>
+      <c r="C556" s="32">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="D556" s="32">
+        <v>72.209999999999994</v>
+      </c>
+      <c r="E556" s="32">
+        <v>68.39</v>
+      </c>
+      <c r="F556" s="32">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="G556" s="32">
+        <v>81.27</v>
+      </c>
+      <c r="H556" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.060000000000002</v>
+      </c>
+      <c r="I556">
+        <f t="shared" si="17"/>
+        <v>-16.896000000000001</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A557" s="33">
+        <v>45331</v>
+      </c>
+      <c r="B557" s="32">
+        <v>72.78</v>
+      </c>
+      <c r="C557" s="32">
+        <v>64.77</v>
+      </c>
+      <c r="D557" s="32">
+        <v>72.78</v>
+      </c>
+      <c r="E557" s="32">
+        <v>68.959999999999994</v>
+      </c>
+      <c r="F557" s="32">
+        <v>64.77</v>
+      </c>
+      <c r="G557" s="32">
+        <v>81.73</v>
+      </c>
+      <c r="H557" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.960000000000008</v>
+      </c>
+      <c r="I557">
+        <f t="shared" si="17"/>
+        <v>-16.93</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A558" s="33">
+        <v>45334</v>
+      </c>
+      <c r="B558" s="32">
+        <v>73.02</v>
+      </c>
+      <c r="C558" s="32">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="D558" s="32">
+        <v>73.02</v>
+      </c>
+      <c r="E558" s="32">
+        <v>69.2</v>
+      </c>
+      <c r="F558" s="32">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="G558" s="32">
+        <v>82</v>
+      </c>
+      <c r="H558" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.930000000000007</v>
+      </c>
+      <c r="I558">
+        <f t="shared" si="17"/>
+        <v>-16.96</v>
+      </c>
+    </row>
+    <row r="559" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A559" s="33">
+        <v>45335</v>
+      </c>
+      <c r="B559" s="32">
+        <v>73.92</v>
+      </c>
+      <c r="C559" s="32">
+        <v>65.91</v>
+      </c>
+      <c r="D559" s="32">
+        <v>73.92</v>
+      </c>
+      <c r="E559" s="32">
+        <v>70.06</v>
+      </c>
+      <c r="F559" s="32">
+        <v>65.91</v>
+      </c>
+      <c r="G559" s="32">
+        <v>82.95</v>
+      </c>
+      <c r="H559" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.040000000000006</v>
+      </c>
+      <c r="I559">
+        <f t="shared" si="17"/>
+        <v>-16.96</v>
+      </c>
+    </row>
+    <row r="560" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A560" s="33">
+        <v>45336</v>
+      </c>
+      <c r="B560" s="32">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="C560" s="32">
+        <v>66.7</v>
+      </c>
+      <c r="D560" s="32">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="E560" s="32">
+        <v>69.81</v>
+      </c>
+      <c r="F560" s="32">
+        <v>66.7</v>
+      </c>
+      <c r="G560" s="32">
+        <v>82.42</v>
+      </c>
+      <c r="H560" s="4">
+        <f t="shared" si="16"/>
+        <v>-15.719999999999999</v>
+      </c>
+      <c r="I560">
+        <f t="shared" si="17"/>
+        <v>-16.742000000000001</v>
+      </c>
+    </row>
+    <row r="561" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A561" s="33">
+        <v>45337</v>
+      </c>
+      <c r="B561" s="32">
+        <v>74.64</v>
+      </c>
+      <c r="C561" s="32">
+        <v>66.62</v>
+      </c>
+      <c r="D561" s="32">
+        <v>74.64</v>
+      </c>
+      <c r="E561" s="32">
+        <v>70.849999999999994</v>
+      </c>
+      <c r="F561" s="32">
+        <v>66.62</v>
+      </c>
+      <c r="G561" s="32">
+        <v>82.73</v>
+      </c>
+      <c r="H561" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.11</v>
+      </c>
+      <c r="I561">
+        <f t="shared" si="17"/>
+        <v>-16.552</v>
+      </c>
+    </row>
+    <row r="562" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A562" s="33">
+        <v>45338</v>
+      </c>
+      <c r="B562" s="32">
+        <v>75.180000000000007</v>
+      </c>
+      <c r="C562" s="32">
+        <v>67.17</v>
+      </c>
+      <c r="D562" s="32">
+        <v>75.180000000000007</v>
+      </c>
+      <c r="E562" s="32">
+        <v>71.39</v>
+      </c>
+      <c r="F562" s="32">
+        <v>67.17</v>
+      </c>
+      <c r="G562" s="32">
+        <v>83.2</v>
+      </c>
+      <c r="H562" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.03</v>
+      </c>
+      <c r="I562">
+        <f t="shared" si="17"/>
+        <v>-16.366</v>
+      </c>
+    </row>
+    <row r="563" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A563" s="33">
+        <v>45341</v>
+      </c>
+      <c r="B563" s="32">
+        <v>75.819999999999993</v>
+      </c>
+      <c r="C563" s="32">
+        <v>67.81</v>
+      </c>
+      <c r="D563" s="32">
+        <v>75.819999999999993</v>
+      </c>
+      <c r="E563" s="32">
+        <v>72.03</v>
+      </c>
+      <c r="F563" s="32">
+        <v>67.81</v>
+      </c>
+      <c r="G563" s="32">
+        <v>83.54</v>
+      </c>
+      <c r="H563" s="4">
+        <f t="shared" si="16"/>
+        <v>-15.730000000000004</v>
+      </c>
+      <c r="I563">
+        <f t="shared" si="17"/>
+        <v>-16.126000000000001</v>
+      </c>
+    </row>
+    <row r="564" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A564" s="33">
+        <v>45342</v>
+      </c>
+      <c r="B564" s="32">
+        <v>75.08</v>
+      </c>
+      <c r="C564" s="32">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="D564" s="32">
+        <v>75.08</v>
+      </c>
+      <c r="E564" s="32">
+        <v>71.290000000000006</v>
+      </c>
+      <c r="F564" s="32">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="G564" s="32">
+        <v>82.31</v>
+      </c>
+      <c r="H564" s="4">
+        <f t="shared" si="16"/>
+        <v>-15.659999999999997</v>
+      </c>
+      <c r="I564">
+        <f t="shared" si="17"/>
+        <v>-15.85</v>
+      </c>
+    </row>
+    <row r="565" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A565" s="33">
+        <v>45343</v>
+      </c>
+      <c r="B565" s="32">
+        <v>75.069999999999993</v>
+      </c>
+      <c r="C565" s="32">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="D565" s="32">
+        <v>75.069999999999993</v>
+      </c>
+      <c r="E565" s="32">
+        <v>70.86</v>
+      </c>
+      <c r="F565" s="32">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="G565" s="32">
+        <v>82.89</v>
+      </c>
+      <c r="H565" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.239999999999995</v>
+      </c>
+      <c r="I565">
+        <f t="shared" si="17"/>
+        <v>-15.954000000000001</v>
+      </c>
+    </row>
+    <row r="566" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A566" s="33">
+        <v>45344</v>
+      </c>
+      <c r="B566" s="32">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="C566" s="32">
+        <v>67.72</v>
+      </c>
+      <c r="D566" s="32">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="E566" s="32">
+        <v>72.36</v>
+      </c>
+      <c r="F566" s="32">
+        <v>67.72</v>
+      </c>
+      <c r="G566" s="32">
+        <v>83.51</v>
+      </c>
+      <c r="H566" s="4">
+        <f t="shared" si="16"/>
+        <v>-15.790000000000006</v>
+      </c>
+      <c r="I566">
+        <f t="shared" si="17"/>
+        <v>-15.89</v>
+      </c>
+    </row>
+    <row r="567" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A567" s="33">
+        <v>45345</v>
+      </c>
+      <c r="B567" s="32">
+        <v>74.44</v>
+      </c>
+      <c r="C567" s="32">
+        <v>66.05</v>
+      </c>
+      <c r="D567" s="32">
+        <v>74.44</v>
+      </c>
+      <c r="E567" s="32">
+        <v>70.239999999999995</v>
+      </c>
+      <c r="F567" s="32">
+        <v>66.05</v>
+      </c>
+      <c r="G567" s="32">
+        <v>82.42</v>
+      </c>
+      <c r="H567" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.370000000000005</v>
+      </c>
+      <c r="I567">
+        <f t="shared" si="17"/>
+        <v>-15.958</v>
+      </c>
+    </row>
+    <row r="568" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A568" s="33">
+        <v>45348</v>
+      </c>
+      <c r="B568" s="32">
+        <v>74.27</v>
+      </c>
+      <c r="C568" s="32">
+        <v>65.89</v>
+      </c>
+      <c r="D568" s="32">
+        <v>74.27</v>
+      </c>
+      <c r="E568" s="32">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="F568" s="32">
+        <v>65.89</v>
+      </c>
+      <c r="G568" s="32">
+        <v>82.26</v>
+      </c>
+      <c r="H568" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.370000000000005</v>
+      </c>
+      <c r="I568">
+        <f t="shared" si="17"/>
+        <v>-16.085999999999999</v>
+      </c>
+    </row>
+    <row r="569" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A569" s="33">
+        <v>45349</v>
+      </c>
+      <c r="B569" s="32">
+        <v>73.819999999999993</v>
+      </c>
+      <c r="C569" s="32">
+        <v>65.680000000000007</v>
+      </c>
+      <c r="D569" s="32">
+        <v>73.819999999999993</v>
+      </c>
+      <c r="E569" s="32">
+        <v>69.86</v>
+      </c>
+      <c r="F569" s="32">
+        <v>65.680000000000007</v>
+      </c>
+      <c r="G569" s="32">
+        <v>83.23</v>
+      </c>
+      <c r="H569" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.549999999999997</v>
+      </c>
+      <c r="I569">
+        <f t="shared" si="17"/>
+        <v>-16.463999999999999</v>
+      </c>
+    </row>
+    <row r="570" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A570" s="33">
+        <v>45350</v>
+      </c>
+      <c r="B570" s="32">
+        <v>74.09</v>
+      </c>
+      <c r="C570" s="32">
+        <v>65.959999999999994</v>
+      </c>
+      <c r="D570" s="32">
+        <v>74.09</v>
+      </c>
+      <c r="E570" s="32">
+        <v>70.13</v>
+      </c>
+      <c r="F570" s="32">
+        <v>65.959999999999994</v>
+      </c>
+      <c r="G570" s="32">
+        <v>83.27</v>
+      </c>
+      <c r="H570" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.310000000000002</v>
+      </c>
+      <c r="I570">
+        <f t="shared" si="17"/>
+        <v>-16.678000000000001</v>
+      </c>
+    </row>
+    <row r="571" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A571" s="33">
+        <v>45351</v>
+      </c>
+      <c r="B571" s="32">
+        <v>74.59</v>
+      </c>
+      <c r="C571" s="32">
+        <v>66.45</v>
+      </c>
+      <c r="D571" s="32">
+        <v>74.59</v>
+      </c>
+      <c r="E571" s="32">
+        <v>70.459999999999994</v>
+      </c>
+      <c r="F571" s="32">
+        <v>66.45</v>
+      </c>
+      <c r="G571" s="32">
+        <v>83.78</v>
+      </c>
+      <c r="H571" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.329999999999998</v>
+      </c>
+      <c r="I571">
+        <f t="shared" si="17"/>
+        <v>-16.986000000000001</v>
+      </c>
+    </row>
+    <row r="572" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A572" s="33">
+        <v>45352</v>
+      </c>
+      <c r="B572" s="32">
+        <v>74.84</v>
+      </c>
+      <c r="C572" s="32">
+        <v>67.39</v>
+      </c>
+      <c r="D572" s="32">
+        <v>74.84</v>
+      </c>
+      <c r="E572" s="32">
+        <v>70.709999999999994</v>
+      </c>
+      <c r="F572" s="32">
+        <v>67.39</v>
+      </c>
+      <c r="G572" s="32">
+        <v>84.19</v>
+      </c>
+      <c r="H572" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.799999999999997</v>
+      </c>
+      <c r="I572">
+        <f t="shared" si="17"/>
+        <v>-17.071999999999999</v>
+      </c>
+    </row>
+    <row r="573" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A573" s="33">
+        <v>45355</v>
+      </c>
+      <c r="B573" s="32">
+        <v>77.83</v>
+      </c>
+      <c r="C573" s="32">
+        <v>69.16</v>
+      </c>
+      <c r="D573" s="32">
+        <v>77.83</v>
+      </c>
+      <c r="E573" s="32">
+        <v>72.95</v>
+      </c>
+      <c r="F573" s="32">
+        <v>69.16</v>
+      </c>
+      <c r="G573" s="32">
+        <v>83.23</v>
+      </c>
+      <c r="H573" s="4">
+        <f t="shared" si="16"/>
+        <v>-14.070000000000007</v>
+      </c>
+      <c r="I573">
+        <f t="shared" si="17"/>
+        <v>-16.611999999999998</v>
+      </c>
+    </row>
+    <row r="574" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A574" s="33">
+        <v>45356</v>
+      </c>
+      <c r="B574" s="32">
+        <v>77.08</v>
+      </c>
+      <c r="C574" s="32">
+        <v>68.42</v>
+      </c>
+      <c r="D574" s="32">
+        <v>77.08</v>
+      </c>
+      <c r="E574" s="32">
+        <v>72.14</v>
+      </c>
+      <c r="F574" s="32">
+        <v>68.42</v>
+      </c>
+      <c r="G574" s="32">
+        <v>82.88</v>
+      </c>
+      <c r="H574" s="4">
+        <f t="shared" si="16"/>
+        <v>-14.459999999999994</v>
+      </c>
+      <c r="I574">
+        <f t="shared" si="17"/>
+        <v>-15.994</v>
+      </c>
+    </row>
+    <row r="575" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A575" s="33">
+        <v>45357</v>
+      </c>
+      <c r="B575" s="32">
+        <v>77.86</v>
+      </c>
+      <c r="C575" s="32">
+        <v>69.19</v>
+      </c>
+      <c r="D575" s="32">
+        <v>77.86</v>
+      </c>
+      <c r="E575" s="32">
+        <v>72.91</v>
+      </c>
+      <c r="F575" s="32">
+        <v>69.19</v>
+      </c>
+      <c r="G575" s="32">
+        <v>84.08</v>
+      </c>
+      <c r="H575" s="4">
+        <f t="shared" si="16"/>
+        <v>-14.89</v>
+      </c>
+      <c r="I575">
+        <f t="shared" si="17"/>
+        <v>-15.51</v>
+      </c>
+    </row>
+    <row r="576" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A576" s="33">
+        <v>45358</v>
+      </c>
+      <c r="B576" s="32">
+        <v>76.14</v>
+      </c>
+      <c r="C576" s="32">
+        <v>69.19</v>
+      </c>
+      <c r="D576" s="32">
+        <v>76.14</v>
+      </c>
+      <c r="E576" s="32">
+        <v>71.19</v>
+      </c>
+      <c r="F576" s="32">
+        <v>69.19</v>
+      </c>
+      <c r="G576" s="32">
+        <v>82.91</v>
+      </c>
+      <c r="H576" s="4">
+        <f t="shared" si="16"/>
+        <v>-13.719999999999999</v>
+      </c>
+      <c r="I576">
+        <f t="shared" si="17"/>
+        <v>-14.788</v>
+      </c>
+    </row>
+    <row r="577" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A577" s="33">
+        <v>45359</v>
+      </c>
+      <c r="B577" s="32">
+        <v>75.52</v>
+      </c>
+      <c r="C577" s="32">
+        <v>66.86</v>
+      </c>
+      <c r="D577" s="32">
+        <v>75.52</v>
+      </c>
+      <c r="E577" s="32">
+        <v>70.569999999999993</v>
+      </c>
+      <c r="F577" s="32">
+        <v>66.86</v>
+      </c>
+      <c r="G577" s="32">
+        <v>82.18</v>
+      </c>
+      <c r="H577" s="4">
+        <f t="shared" si="16"/>
+        <v>-15.320000000000007</v>
+      </c>
+      <c r="I577">
+        <f t="shared" si="17"/>
+        <v>-14.492000000000001</v>
+      </c>
+    </row>
+    <row r="578" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A578" s="33">
+        <v>45362</v>
+      </c>
+      <c r="B578" s="32">
+        <v>74.7</v>
+      </c>
+      <c r="C578" s="32">
+        <v>66.010000000000005</v>
+      </c>
+      <c r="D578" s="32">
+        <v>74.7</v>
+      </c>
+      <c r="E578" s="32">
+        <v>69.72</v>
+      </c>
+      <c r="F578" s="32">
+        <v>66.010000000000005</v>
+      </c>
+      <c r="G578" s="32">
+        <v>82.63</v>
+      </c>
+      <c r="H578" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.61999999999999</v>
+      </c>
+      <c r="I578">
+        <f t="shared" si="17"/>
+        <v>-15.002000000000001</v>
+      </c>
+    </row>
+    <row r="579" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A579" s="33">
+        <v>45363</v>
+      </c>
+      <c r="B579" s="32">
+        <v>74.92</v>
+      </c>
+      <c r="C579" s="32">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="D579" s="32">
+        <v>74.92</v>
+      </c>
+      <c r="E579" s="32">
+        <v>69.94</v>
+      </c>
+      <c r="F579" s="32">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="G579" s="32">
+        <v>82.55</v>
+      </c>
+      <c r="H579" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.36999999999999</v>
+      </c>
+      <c r="I579">
+        <f t="shared" si="17"/>
+        <v>-15.384</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A580" s="33">
+        <v>45364</v>
+      </c>
+      <c r="B580" s="32">
+        <v>75.180000000000007</v>
+      </c>
+      <c r="C580" s="32">
+        <v>66.52</v>
+      </c>
+      <c r="D580" s="32">
+        <v>75.180000000000007</v>
+      </c>
+      <c r="E580" s="32">
+        <v>70.28</v>
+      </c>
+      <c r="F580" s="32">
+        <v>66.52</v>
+      </c>
+      <c r="G580" s="32">
+        <v>83.61</v>
+      </c>
+      <c r="H580" s="4">
+        <f t="shared" si="16"/>
+        <v>-17.090000000000003</v>
+      </c>
+      <c r="I580">
+        <f t="shared" si="17"/>
+        <v>-15.824</v>
+      </c>
+    </row>
+    <row r="581" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A581" s="33">
+        <v>45365</v>
+      </c>
+      <c r="B581" s="32">
+        <v>77.39</v>
+      </c>
+      <c r="C581" s="32">
+        <v>68.73</v>
+      </c>
+      <c r="D581" s="32">
+        <v>77.39</v>
+      </c>
+      <c r="E581" s="32">
+        <v>72.540000000000006</v>
+      </c>
+      <c r="F581" s="32">
+        <v>68.73</v>
+      </c>
+      <c r="G581" s="32">
+        <v>85.2</v>
+      </c>
+      <c r="H581" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.47</v>
+      </c>
+      <c r="I581">
+        <f t="shared" si="17"/>
+        <v>-16.373999999999999</v>
+      </c>
+    </row>
+    <row r="582" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A582" s="33">
+        <v>45366</v>
+      </c>
+      <c r="B582" s="32">
+        <v>76.62</v>
+      </c>
+      <c r="C582" s="32">
+        <v>68.73</v>
+      </c>
+      <c r="D582" s="32">
+        <v>76.62</v>
+      </c>
+      <c r="E582" s="32">
+        <v>71.77</v>
+      </c>
+      <c r="F582" s="32">
+        <v>68.73</v>
+      </c>
+      <c r="G582" s="32">
+        <v>85.44</v>
+      </c>
+      <c r="H582" s="4">
+        <f t="shared" si="16"/>
+        <v>-16.709999999999994</v>
+      </c>
+      <c r="I582">
+        <f t="shared" si="17"/>
+        <v>-16.652000000000001</v>
+      </c>
+    </row>
+    <row r="583" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A583" s="33">
+        <v>45369</v>
+      </c>
+      <c r="B583" s="32">
+        <v>77.7</v>
+      </c>
+      <c r="C583" s="32">
+        <v>67.959999999999994</v>
+      </c>
+      <c r="D583" s="32">
+        <v>77.7</v>
+      </c>
+      <c r="E583" s="32">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="F583" s="32">
+        <v>67.959999999999994</v>
+      </c>
+      <c r="G583" s="32">
+        <v>86.49</v>
+      </c>
+      <c r="H583" s="4">
+        <f t="shared" si="16"/>
+        <v>-18.53</v>
+      </c>
+      <c r="I583">
+        <f t="shared" si="17"/>
+        <v>-17.033999999999999</v>
+      </c>
+    </row>
+    <row r="584" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A584" s="33">
+        <v>45370</v>
+      </c>
+      <c r="B584" s="32">
+        <v>78.59</v>
+      </c>
+      <c r="C584" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="D584" s="32">
+        <v>78.59</v>
+      </c>
+      <c r="E584" s="32">
+        <v>73.88</v>
+      </c>
+      <c r="F584" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="G584" s="32">
+        <v>87.39</v>
+      </c>
+      <c r="H584" s="4">
+        <f t="shared" si="16"/>
+        <v>-18.349999999999994</v>
+      </c>
+      <c r="I584">
+        <f t="shared" si="17"/>
+        <v>-17.43</v>
+      </c>
+    </row>
+    <row r="585" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A585" s="33">
+        <v>45371</v>
+      </c>
+      <c r="B585" s="32">
+        <v>77</v>
+      </c>
+      <c r="C585" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="D585" s="32">
+        <v>77</v>
+      </c>
+      <c r="E585" s="32">
+        <v>72.319999999999993</v>
+      </c>
+      <c r="F585" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="G585" s="32">
+        <v>85.99</v>
+      </c>
+      <c r="H585" s="4">
+        <f t="shared" ref="H585:H599" si="18">AVERAGE(C585,F585)-G585</f>
+        <v>-16.949999999999989</v>
+      </c>
+      <c r="I585">
+        <f t="shared" ref="I585:I599" si="19" xml:space="preserve"> ROUND(AVERAGE(H581:H585), 3)</f>
+        <v>-17.402000000000001</v>
+      </c>
+    </row>
+    <row r="586" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A586" s="33">
+        <v>45372</v>
+      </c>
+      <c r="B586" s="32">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="C586" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="D586" s="32">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="E586" s="32">
+        <v>71.47</v>
+      </c>
+      <c r="F586" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="G586" s="32">
+        <v>85.56</v>
+      </c>
+      <c r="H586" s="4">
+        <f t="shared" si="18"/>
+        <v>-16.519999999999996</v>
+      </c>
+      <c r="I586">
+        <f t="shared" si="19"/>
+        <v>-17.411999999999999</v>
+      </c>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A587" s="33">
+        <v>45373</v>
+      </c>
+      <c r="B587" s="32">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="C587" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="D587" s="32">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="E587" s="32">
+        <v>71.42</v>
+      </c>
+      <c r="F587" s="32">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="G587" s="32">
+        <v>85.58</v>
+      </c>
+      <c r="H587" s="4">
+        <f t="shared" si="18"/>
+        <v>-16.539999999999992</v>
+      </c>
+      <c r="I587">
+        <f t="shared" si="19"/>
+        <v>-17.378</v>
+      </c>
+    </row>
+    <row r="588" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A588" s="33">
+        <v>45376</v>
+      </c>
+      <c r="B588" s="32">
+        <v>77.41</v>
+      </c>
+      <c r="C588" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="D588" s="32">
+        <v>77.41</v>
+      </c>
+      <c r="E588" s="32">
+        <v>72.73</v>
+      </c>
+      <c r="F588" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="G588" s="32">
+        <v>86.88</v>
+      </c>
+      <c r="H588" s="4">
+        <f t="shared" si="18"/>
+        <v>-19.439999999999998</v>
+      </c>
+      <c r="I588">
+        <f t="shared" si="19"/>
+        <v>-17.559999999999999</v>
+      </c>
+    </row>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A589" s="33">
+        <v>45377</v>
+      </c>
+      <c r="B589" s="32">
+        <v>77.17</v>
+      </c>
+      <c r="C589" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="D589" s="32">
+        <v>77.17</v>
+      </c>
+      <c r="E589" s="32">
+        <v>72.459999999999994</v>
+      </c>
+      <c r="F589" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="G589" s="32">
+        <v>86.62</v>
+      </c>
+      <c r="H589" s="4">
+        <f t="shared" si="18"/>
+        <v>-19.180000000000007</v>
+      </c>
+      <c r="I589">
+        <f t="shared" si="19"/>
+        <v>-17.725999999999999</v>
+      </c>
+    </row>
+    <row r="590" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A590" s="33">
+        <v>45378</v>
+      </c>
+      <c r="B590" s="32">
+        <v>76.2</v>
+      </c>
+      <c r="C590" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="D590" s="32">
+        <v>76.2</v>
+      </c>
+      <c r="E590" s="32">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="F590" s="32">
+        <v>67.44</v>
+      </c>
+      <c r="G590" s="32">
+        <v>85.94</v>
+      </c>
+      <c r="H590" s="4">
+        <f t="shared" si="18"/>
+        <v>-18.5</v>
+      </c>
+      <c r="I590">
+        <f t="shared" si="19"/>
+        <v>-18.036000000000001</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A591" s="33">
+        <v>45379</v>
+      </c>
+      <c r="B591" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="C591" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="D591" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="E591" s="32">
+        <v>72.72</v>
+      </c>
+      <c r="F591" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="G591" s="32">
+        <v>87.42</v>
+      </c>
+      <c r="H591" s="4">
+        <f t="shared" si="18"/>
+        <v>-18.650000000000006</v>
+      </c>
+      <c r="I591">
+        <f t="shared" si="19"/>
+        <v>-18.462</v>
+      </c>
+    </row>
+    <row r="592" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A592" s="33">
+        <v>45380</v>
+      </c>
+      <c r="B592" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="C592" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="D592" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="E592" s="32">
+        <v>72.72</v>
+      </c>
+      <c r="F592" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="G592" s="32">
+        <v>87.42</v>
+      </c>
+      <c r="H592" s="4">
+        <f t="shared" si="18"/>
+        <v>-18.650000000000006</v>
+      </c>
+      <c r="I592">
+        <f t="shared" si="19"/>
+        <v>-18.884</v>
+      </c>
+    </row>
+    <row r="593" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A593" s="33">
+        <v>45383</v>
+      </c>
+      <c r="B593" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="C593" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="D593" s="32">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="E593" s="32">
+        <v>72.72</v>
+      </c>
+      <c r="F593" s="32">
+        <v>68.77</v>
+      </c>
+      <c r="G593" s="32">
+        <v>87.42</v>
+      </c>
+      <c r="H593" s="4">
+        <f t="shared" si="18"/>
+        <v>-18.650000000000006</v>
+      </c>
+      <c r="I593">
+        <f t="shared" si="19"/>
+        <v>-18.725999999999999</v>
+      </c>
+    </row>
+    <row r="594" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A594" s="33">
+        <v>45384</v>
+      </c>
+      <c r="B594" s="32">
+        <v>78.89</v>
+      </c>
+      <c r="C594" s="32">
+        <v>70.27</v>
+      </c>
+      <c r="D594" s="32">
+        <v>78.89</v>
+      </c>
+      <c r="E594" s="32">
+        <v>74.180000000000007</v>
+      </c>
+      <c r="F594" s="32">
+        <v>70.27</v>
+      </c>
+      <c r="G594" s="32">
+        <v>88.9</v>
+      </c>
+      <c r="H594" s="4">
+        <f t="shared" si="18"/>
+        <v>-18.63000000000001</v>
+      </c>
+      <c r="I594">
+        <f t="shared" si="19"/>
+        <v>-18.616</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A595" s="33">
+        <v>45385</v>
+      </c>
+      <c r="B595" s="32">
+        <v>81.84</v>
+      </c>
+      <c r="C595" s="32">
+        <v>73.27</v>
+      </c>
+      <c r="D595" s="32">
+        <v>81.84</v>
+      </c>
+      <c r="E595" s="32">
+        <v>77.13</v>
+      </c>
+      <c r="F595" s="32">
+        <v>73.27</v>
+      </c>
+      <c r="G595" s="32">
+        <v>89.78</v>
+      </c>
+      <c r="H595" s="4">
+        <f t="shared" si="18"/>
+        <v>-16.510000000000005</v>
+      </c>
+      <c r="I595">
+        <f t="shared" si="19"/>
+        <v>-18.218</v>
+      </c>
+    </row>
+    <row r="596" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A596" s="33">
+        <v>45386</v>
+      </c>
+      <c r="B596" s="32">
+        <v>81.58</v>
+      </c>
+      <c r="C596" s="32">
+        <v>72.89</v>
+      </c>
+      <c r="D596" s="32">
+        <v>81.58</v>
+      </c>
+      <c r="E596" s="32">
+        <v>76.87</v>
+      </c>
+      <c r="F596" s="32">
+        <v>72.89</v>
+      </c>
+      <c r="G596" s="32">
+        <v>89.23</v>
+      </c>
+      <c r="H596" s="4">
+        <f t="shared" si="18"/>
+        <v>-16.340000000000003</v>
+      </c>
+      <c r="I596">
+        <f t="shared" si="19"/>
+        <v>-17.756</v>
+      </c>
+    </row>
+    <row r="597" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A597" s="33">
+        <v>45387</v>
+      </c>
+      <c r="B597" s="32">
+        <v>84.07</v>
+      </c>
+      <c r="C597" s="32">
+        <v>75.38</v>
+      </c>
+      <c r="D597" s="32">
+        <v>84.07</v>
+      </c>
+      <c r="E597" s="32">
+        <v>79.19</v>
+      </c>
+      <c r="F597" s="32">
+        <v>75.38</v>
+      </c>
+      <c r="G597" s="32">
+        <v>91.55</v>
+      </c>
+      <c r="H597" s="4">
+        <f t="shared" si="18"/>
+        <v>-16.170000000000002</v>
+      </c>
+      <c r="I597">
+        <f t="shared" si="19"/>
+        <v>-17.260000000000002</v>
+      </c>
+    </row>
+    <row r="598" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A598" s="33">
+        <v>45390</v>
+      </c>
+      <c r="B598" s="32">
+        <v>82.99</v>
+      </c>
+      <c r="C598" s="32">
+        <v>74.3</v>
+      </c>
+      <c r="D598" s="32">
+        <v>82.99</v>
+      </c>
+      <c r="E598" s="32">
+        <v>78.11</v>
+      </c>
+      <c r="F598" s="32">
+        <v>74.3</v>
+      </c>
+      <c r="G598" s="32">
+        <v>89.95</v>
+      </c>
+      <c r="H598" s="4">
+        <f t="shared" si="18"/>
+        <v>-15.650000000000006</v>
+      </c>
+      <c r="I598">
+        <f t="shared" si="19"/>
+        <v>-16.66</v>
+      </c>
+    </row>
+    <row r="599" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A599" s="33">
+        <v>45391</v>
+      </c>
+      <c r="B599" s="32">
+        <v>83.39</v>
+      </c>
+      <c r="C599" s="32">
+        <v>74.3</v>
+      </c>
+      <c r="D599" s="32">
+        <v>83.39</v>
+      </c>
+      <c r="E599" s="32">
+        <v>78.510000000000005</v>
+      </c>
+      <c r="F599" s="32">
+        <v>74.3</v>
+      </c>
+      <c r="G599" s="32">
+        <v>89.92</v>
+      </c>
+      <c r="H599" s="4">
+        <f t="shared" si="18"/>
+        <v>-15.620000000000005</v>
+      </c>
+      <c r="I599">
+        <f t="shared" si="19"/>
+        <v>-16.058</v>
+      </c>
+    </row>
+    <row r="600" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B600" s="32"/>
+      <c r="C600" s="32"/>
+      <c r="D600" s="32"/>
+      <c r="E600" s="32"/>
+      <c r="F600" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>